<commit_message>
Implemented concurrent execution of data_analysis/ helper scripts
</commit_message>
<xml_diff>
--- a/data_analysis/elasticity/elasticity.xlsx
+++ b/data_analysis/elasticity/elasticity.xlsx
@@ -709,7 +709,7 @@
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -731,7 +731,7 @@
         <v>271</v>
       </c>
       <c r="C2" s="3">
-        <v>1.35725631402635</v>
+        <v>1.357256314026351</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -742,7 +742,7 @@
         <v>354.6111111111111</v>
       </c>
       <c r="C3" s="3">
-        <v>6.887094143371944</v>
+        <v>6.887094143371947</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -753,7 +753,7 @@
         <v>1695.222222222222</v>
       </c>
       <c r="C4" s="3">
-        <v>0.9621589682907417</v>
+        <v>0.9621589682907425</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -764,7 +764,7 @@
         <v>575.1176470588235</v>
       </c>
       <c r="C5" s="3">
-        <v>3.945005804783354</v>
+        <v>3.945005804783356</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -775,7 +775,7 @@
         <v>1770.055555555556</v>
       </c>
       <c r="C6" s="3">
-        <v>3.998255047180202</v>
+        <v>3.998255047180205</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -786,7 +786,7 @@
         <v>1510.111111111111</v>
       </c>
       <c r="C7" s="3">
-        <v>4.546150634098066</v>
+        <v>4.546150634098068</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -797,7 +797,7 @@
         <v>543.2777777777778</v>
       </c>
       <c r="C8" s="3">
-        <v>3.8898703995655</v>
+        <v>3.889870399565503</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -808,7 +808,7 @@
         <v>12698.77777777778</v>
       </c>
       <c r="C9" s="3">
-        <v>1.783866583660905</v>
+        <v>1.783866583660906</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -819,7 +819,7 @@
         <v>1719.277777777778</v>
       </c>
       <c r="C10" s="3">
-        <v>-0.03230382618528604</v>
+        <v>-0.0323038261852856</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -830,7 +830,7 @@
         <v>4388.333333333333</v>
       </c>
       <c r="C11" s="3">
-        <v>3.154566206059836</v>
+        <v>3.154566206059838</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -841,7 +841,7 @@
         <v>1215.833333333333</v>
       </c>
       <c r="C12" s="3">
-        <v>4.520087914571928</v>
+        <v>4.52008791457193</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -852,7 +852,7 @@
         <v>1003.333333333333</v>
       </c>
       <c r="C13" s="3">
-        <v>2.327125813468714</v>
+        <v>2.327125813468715</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -863,7 +863,7 @@
         <v>966.9444444444445</v>
       </c>
       <c r="C14" s="3">
-        <v>3.633383811351338</v>
+        <v>3.63338381135134</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -874,7 +874,7 @@
         <v>2408.055555555556</v>
       </c>
       <c r="C15" s="3">
-        <v>1.940028840493857</v>
+        <v>1.940028840493859</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -885,7 +885,7 @@
         <v>704.5</v>
       </c>
       <c r="C16" s="3">
-        <v>2.838654908492098</v>
+        <v>2.838654908492099</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -896,7 +896,7 @@
         <v>645.2777777777778</v>
       </c>
       <c r="C17" s="3">
-        <v>0.8796179759578735</v>
+        <v>0.8796179759578744</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -907,7 +907,7 @@
         <v>7539.722222222223</v>
       </c>
       <c r="C18" s="3">
-        <v>2.369143003552924</v>
+        <v>2.369143003552927</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -918,7 +918,7 @@
         <v>366.0555555555555</v>
       </c>
       <c r="C19" s="3">
-        <v>5.145604421258335</v>
+        <v>5.145604421258338</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -929,7 +929,7 @@
         <v>2289.888888888889</v>
       </c>
       <c r="C20" s="3">
-        <v>2.114770802958085</v>
+        <v>2.114770802958087</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -940,7 +940,7 @@
         <v>4304.722222222223</v>
       </c>
       <c r="C21" s="3">
-        <v>2.060478459612275</v>
+        <v>2.060478459612276</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -951,7 +951,7 @@
         <v>540.8888888888889</v>
       </c>
       <c r="C22" s="3">
-        <v>2.262430506182488</v>
+        <v>2.262430506182489</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -962,7 +962,7 @@
         <v>1404.611111111111</v>
       </c>
       <c r="C23" s="3">
-        <v>3.339439589950414</v>
+        <v>3.339439589950416</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -973,7 +973,7 @@
         <v>1308.944444444444</v>
       </c>
       <c r="C24" s="3">
-        <v>2.978555887229455</v>
+        <v>2.978555887229456</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -984,7 +984,7 @@
         <v>854.9411764705883</v>
       </c>
       <c r="C25" s="3">
-        <v>2.194402962374678</v>
+        <v>2.194402962374679</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -995,7 +995,7 @@
         <v>3735.055555555556</v>
       </c>
       <c r="C26" s="3">
-        <v>1.624458607049494</v>
+        <v>1.624458607049496</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1006,7 +1006,7 @@
         <v>19142.27777777778</v>
       </c>
       <c r="C27" s="3">
-        <v>0.9990234685779513</v>
+        <v>0.9990234685779522</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1028,7 +1028,7 @@
         <v>1108.333333333333</v>
       </c>
       <c r="C29" s="3">
-        <v>4.37942380018478</v>
+        <v>4.379423800184783</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1039,7 +1039,7 @@
         <v>847.2777777777778</v>
       </c>
       <c r="C30" s="3">
-        <v>2.572031666180989</v>
+        <v>2.57203166618099</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1050,7 +1050,7 @@
         <v>16813.55555555555</v>
       </c>
       <c r="C31" s="3">
-        <v>1.824416770379819</v>
+        <v>1.82441677037982</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1061,7 +1061,7 @@
         <v>1382.111111111111</v>
       </c>
       <c r="C32" s="3">
-        <v>4.898482965635322</v>
+        <v>4.898482965635325</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1072,7 +1072,7 @@
         <v>765.875</v>
       </c>
       <c r="C33" s="3">
-        <v>0.5731196185501</v>
+        <v>0.5731196185501006</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1083,7 +1083,7 @@
         <v>1598.5</v>
       </c>
       <c r="C34" s="3">
-        <v>0.5343369108736038</v>
+        <v>0.5343369108736047</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1094,7 +1094,7 @@
         <v>52043.83333333334</v>
       </c>
       <c r="C35" s="3">
-        <v>0.9589643109472232</v>
+        <v>0.9589643109472241</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1105,7 +1105,7 @@
         <v>721.0555555555555</v>
       </c>
       <c r="C36" s="3">
-        <v>3.327938956505582</v>
+        <v>3.327938956505584</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1116,7 +1116,7 @@
         <v>697</v>
       </c>
       <c r="C37" s="3">
-        <v>1.94581028903611</v>
+        <v>1.945810289036112</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1127,7 +1127,7 @@
         <v>4986.222222222223</v>
       </c>
       <c r="C38" s="3">
-        <v>2.416673700971703</v>
+        <v>2.416673700971705</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1138,7 +1138,7 @@
         <v>5723.611111111111</v>
       </c>
       <c r="C39" s="3">
-        <v>1.509234673336074</v>
+        <v>1.509234673336075</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1149,7 +1149,7 @@
         <v>2469.388888888889</v>
       </c>
       <c r="C40" s="3">
-        <v>2.131539285800402</v>
+        <v>2.131539285800403</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1160,7 +1160,7 @@
         <v>827.3888888888889</v>
       </c>
       <c r="C41" s="3">
-        <v>3.933745317083301</v>
+        <v>3.933745317083303</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1171,7 +1171,7 @@
         <v>4127.166666666667</v>
       </c>
       <c r="C42" s="3">
-        <v>2.115583174554904</v>
+        <v>2.115583174554906</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1182,7 +1182,7 @@
         <v>932</v>
       </c>
       <c r="C43" s="3">
-        <v>1.756911632289728</v>
+        <v>1.756911632289729</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1193,7 +1193,7 @@
         <v>360.1111111111111</v>
       </c>
       <c r="C44" s="3">
-        <v>3.39133184220729</v>
+        <v>3.391331842207292</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1204,7 +1204,7 @@
         <v>1298.388888888889</v>
       </c>
       <c r="C45" s="3">
-        <v>3.176899455564953</v>
+        <v>3.176899455564954</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1215,7 +1215,7 @@
         <v>1161.5</v>
       </c>
       <c r="C46" s="3">
-        <v>4.910995710330457</v>
+        <v>4.91099571033046</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1226,7 +1226,7 @@
         <v>489.0555555555555</v>
       </c>
       <c r="C47" s="3">
-        <v>3.008838168732169</v>
+        <v>3.00883816873217</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1237,7 +1237,7 @@
         <v>1469.222222222222</v>
       </c>
       <c r="C48" s="3">
-        <v>2.720345156539985</v>
+        <v>2.720345156539986</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1248,7 +1248,7 @@
         <v>898.9444444444445</v>
       </c>
       <c r="C49" s="3">
-        <v>8.023132541218956</v>
+        <v>8.023132541218962</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1259,7 +1259,7 @@
         <v>589.5555555555555</v>
       </c>
       <c r="C50" s="3">
-        <v>4.246522363577463</v>
+        <v>4.246522363577466</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1270,7 +1270,7 @@
         <v>1381</v>
       </c>
       <c r="C51" s="3">
-        <v>5.41825371553831</v>
+        <v>5.418253715538313</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1281,7 +1281,7 @@
         <v>198.0555555555555</v>
       </c>
       <c r="C52" s="3">
-        <v>2.114741053280721</v>
+        <v>2.114741053280722</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1292,7 +1292,7 @@
         <v>4762.055555555556</v>
       </c>
       <c r="C53" s="3">
-        <v>3.281235553054098</v>
+        <v>3.2812355530541</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1303,7 +1303,7 @@
         <v>304.5555555555555</v>
       </c>
       <c r="C54" s="3">
-        <v>5.423905213307876</v>
+        <v>5.423905213307879</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1314,7 +1314,7 @@
         <v>2657.555555555556</v>
       </c>
       <c r="C55" s="3">
-        <v>4.197561285620755</v>
+        <v>4.197561285620758</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1325,7 +1325,7 @@
         <v>18208.16666666667</v>
       </c>
       <c r="C56" s="3">
-        <v>1.784736035585024</v>
+        <v>1.784736035585025</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1336,7 +1336,7 @@
         <v>65204.44444444445</v>
       </c>
       <c r="C57" s="3">
-        <v>1.277468593367812</v>
+        <v>1.277468593367814</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1347,7 +1347,7 @@
         <v>1029.5</v>
       </c>
       <c r="C58" s="3">
-        <v>0.9283714397010021</v>
+        <v>0.928371439701003</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1358,7 +1358,7 @@
         <v>4244.111111111111</v>
       </c>
       <c r="C59" s="3">
-        <v>1.952990849728095</v>
+        <v>1.952990849728096</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1369,7 +1369,7 @@
         <v>953.5555555555555</v>
       </c>
       <c r="C60" s="3">
-        <v>4.038286161672137</v>
+        <v>4.03828616167214</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1380,7 +1380,7 @@
         <v>1344.444444444444</v>
       </c>
       <c r="C61" s="3">
-        <v>3.921826183576595</v>
+        <v>3.921826183576597</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1391,7 +1391,7 @@
         <v>1676.388888888889</v>
       </c>
       <c r="C62" s="3">
-        <v>2.591569538840899</v>
+        <v>2.591569538840901</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1402,7 +1402,7 @@
         <v>8862.111111111111</v>
       </c>
       <c r="C63" s="3">
-        <v>1.015540391140557</v>
+        <v>1.015540391140558</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1413,7 +1413,7 @@
         <v>688.2222222222222</v>
       </c>
       <c r="C64" s="3">
-        <v>2.704154469791415</v>
+        <v>2.704154469791416</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1424,7 +1424,7 @@
         <v>1787.444444444444</v>
       </c>
       <c r="C65" s="3">
-        <v>2.554172184965163</v>
+        <v>2.554172184965164</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1435,7 +1435,7 @@
         <v>1955.555555555556</v>
       </c>
       <c r="C66" s="3">
-        <v>3.707019874209061</v>
+        <v>3.707019874209064</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1446,7 +1446,7 @@
         <v>1406.222222222222</v>
       </c>
       <c r="C67" s="3">
-        <v>2.606731384182654</v>
+        <v>2.606731384182656</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1457,7 +1457,7 @@
         <v>1148.666666666667</v>
       </c>
       <c r="C68" s="3">
-        <v>2.96719973826789</v>
+        <v>2.967199738267892</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1468,7 +1468,7 @@
         <v>994.7777777777778</v>
       </c>
       <c r="C69" s="3">
-        <v>5.274725717453601</v>
+        <v>5.274725717453603</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1479,7 +1479,7 @@
         <v>433</v>
       </c>
       <c r="C70" s="3">
-        <v>3.283537035349036</v>
+        <v>3.283537035349038</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1490,7 +1490,7 @@
         <v>15794.88888888889</v>
       </c>
       <c r="C71" s="3">
-        <v>1.732085870349754</v>
+        <v>1.732085870349755</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1501,7 +1501,7 @@
         <v>845.8888888888889</v>
       </c>
       <c r="C72" s="3">
-        <v>1.809890164114266</v>
+        <v>1.809890164114267</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1512,7 +1512,7 @@
         <v>1314.277777777778</v>
       </c>
       <c r="C73" s="3">
-        <v>1.865748618876328</v>
+        <v>1.865748618876329</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1523,7 +1523,7 @@
         <v>360.3333333333333</v>
       </c>
       <c r="C74" s="3">
-        <v>3.257262687746987</v>
+        <v>3.257262687746989</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1534,7 +1534,7 @@
         <v>18092.33333333333</v>
       </c>
       <c r="C75" s="3">
-        <v>2.276943870757617</v>
+        <v>2.276943870757618</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1545,7 +1545,7 @@
         <v>805.1666666666666</v>
       </c>
       <c r="C76" s="3">
-        <v>3.882179446133341</v>
+        <v>3.882179446133343</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1556,7 +1556,7 @@
         <v>1208.611111111111</v>
       </c>
       <c r="C77" s="3">
-        <v>4.085181848712212</v>
+        <v>4.085181848712214</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1567,7 +1567,7 @@
         <v>11635.55555555555</v>
       </c>
       <c r="C78" s="3">
-        <v>1.409696492634694</v>
+        <v>1.409696492634695</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1578,7 +1578,7 @@
         <v>5419</v>
       </c>
       <c r="C79" s="3">
-        <v>1.173257410267234</v>
+        <v>1.173257410267235</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1589,7 +1589,7 @@
         <v>1820.388888888889</v>
       </c>
       <c r="C80" s="3">
-        <v>0.571311153813002</v>
+        <v>0.5713111538130027</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1600,7 +1600,7 @@
         <v>1480.333333333333</v>
       </c>
       <c r="C81" s="3">
-        <v>1.692927509218713</v>
+        <v>1.692927509218714</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1622,7 +1622,7 @@
         <v>426.5</v>
       </c>
       <c r="C83" s="3">
-        <v>4.635793554937599</v>
+        <v>4.635793554937601</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1633,7 +1633,7 @@
         <v>1599.111111111111</v>
       </c>
       <c r="C84" s="3">
-        <v>2.981145719466401</v>
+        <v>2.981145719466403</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1644,7 +1644,7 @@
         <v>565.0588235294117</v>
       </c>
       <c r="C85" s="3">
-        <v>2.264175256123465</v>
+        <v>2.264175256123466</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1655,7 +1655,7 @@
         <v>246.4117647058823</v>
       </c>
       <c r="C86" s="3">
-        <v>1.158124226992246</v>
+        <v>1.158124226992247</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1666,7 +1666,7 @@
         <v>812.8333333333334</v>
       </c>
       <c r="C87" s="3">
-        <v>3.336739651606498</v>
+        <v>3.336739651606501</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1677,7 +1677,7 @@
         <v>950.3333333333334</v>
       </c>
       <c r="C88" s="3">
-        <v>2.968406732834274</v>
+        <v>2.968406732834276</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1688,7 +1688,7 @@
         <v>718.3333333333334</v>
       </c>
       <c r="C89" s="3">
-        <v>7.020103735428291</v>
+        <v>7.020103735428295</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1699,7 +1699,7 @@
         <v>1363.166666666667</v>
       </c>
       <c r="C90" s="3">
-        <v>3.418821882174067</v>
+        <v>3.418821882174068</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1710,7 +1710,7 @@
         <v>2240.222222222222</v>
       </c>
       <c r="C91" s="3">
-        <v>3.08706349343197</v>
+        <v>3.087063493431971</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1721,7 +1721,7 @@
         <v>1087.055555555556</v>
       </c>
       <c r="C92" s="3">
-        <v>4.759575287918111</v>
+        <v>4.759575287918112</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1732,7 +1732,7 @@
         <v>1021.222222222222</v>
       </c>
       <c r="C93" s="3">
-        <v>6.007627490035411</v>
+        <v>6.007627490035413</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1743,7 +1743,7 @@
         <v>2075.555555555556</v>
       </c>
       <c r="C94" s="3">
-        <v>2.260271692479443</v>
+        <v>2.260271692479445</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1754,7 +1754,7 @@
         <v>5576.888888888889</v>
       </c>
       <c r="C95" s="3">
-        <v>1.586326401123529</v>
+        <v>1.58632640112353</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1765,7 +1765,7 @@
         <v>2741.777777777778</v>
       </c>
       <c r="C96" s="3">
-        <v>1.826592004438217</v>
+        <v>1.826592004438218</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1776,7 +1776,7 @@
         <v>349.6666666666667</v>
       </c>
       <c r="C97" s="3">
-        <v>2.678940404510244</v>
+        <v>2.678940404510246</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1787,7 +1787,7 @@
         <v>4738.722222222223</v>
       </c>
       <c r="C98" s="3">
-        <v>2.020898137479048</v>
+        <v>2.02089813747905</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1798,7 +1798,7 @@
         <v>429.7222222222222</v>
       </c>
       <c r="C99" s="3">
-        <v>2.454632666991825</v>
+        <v>2.454632666991827</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1809,7 +1809,7 @@
         <v>4262.444444444444</v>
       </c>
       <c r="C100" s="3">
-        <v>1.518729168682847</v>
+        <v>1.518729168682849</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1820,7 +1820,7 @@
         <v>1411.222222222222</v>
       </c>
       <c r="C101" s="3">
-        <v>2.741347663741911</v>
+        <v>2.741347663741912</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1831,7 +1831,7 @@
         <v>1071.666666666667</v>
       </c>
       <c r="C102" s="3">
-        <v>3.382878491978183</v>
+        <v>3.382878491978186</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1842,7 +1842,7 @@
         <v>4690</v>
       </c>
       <c r="C103" s="3">
-        <v>1.939948131515448</v>
+        <v>1.939948131515449</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1853,7 +1853,7 @@
         <v>610.0555555555555</v>
       </c>
       <c r="C104" s="3">
-        <v>4.675489641386824</v>
+        <v>4.675489641386827</v>
       </c>
     </row>
     <row r="105" spans="1:3">

</xml_diff>

<commit_message>
Redid CRE; added CRE-2SLS; updated data report
</commit_message>
<xml_diff>
--- a/data_analysis/elasticity/elasticity.xlsx
+++ b/data_analysis/elasticity/elasticity.xlsx
@@ -709,7 +709,7 @@
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -731,7 +731,7 @@
         <v>271</v>
       </c>
       <c r="C2" s="3">
-        <v>1.357256314026351</v>
+        <v>1.35725631402635</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -742,7 +742,7 @@
         <v>354.6111111111111</v>
       </c>
       <c r="C3" s="3">
-        <v>6.887094143371947</v>
+        <v>6.887094143371946</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -753,7 +753,7 @@
         <v>1695.222222222222</v>
       </c>
       <c r="C4" s="3">
-        <v>0.9621589682907425</v>
+        <v>0.9621589682907421</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -764,7 +764,7 @@
         <v>575.1176470588235</v>
       </c>
       <c r="C5" s="3">
-        <v>3.945005804783356</v>
+        <v>3.945005804783355</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -775,7 +775,7 @@
         <v>1770.055555555556</v>
       </c>
       <c r="C6" s="3">
-        <v>3.998255047180205</v>
+        <v>3.998255047180203</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -786,7 +786,7 @@
         <v>1510.111111111111</v>
       </c>
       <c r="C7" s="3">
-        <v>4.546150634098068</v>
+        <v>4.546150634098067</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -797,7 +797,7 @@
         <v>543.2777777777778</v>
       </c>
       <c r="C8" s="3">
-        <v>3.889870399565503</v>
+        <v>3.889870399565502</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -808,7 +808,7 @@
         <v>12698.77777777778</v>
       </c>
       <c r="C9" s="3">
-        <v>1.783866583660906</v>
+        <v>1.783866583660905</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -819,7 +819,7 @@
         <v>1719.277777777778</v>
       </c>
       <c r="C10" s="3">
-        <v>-0.0323038261852856</v>
+        <v>-0.03230382618528582</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -830,7 +830,7 @@
         <v>4388.333333333333</v>
       </c>
       <c r="C11" s="3">
-        <v>3.154566206059838</v>
+        <v>3.154566206059837</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -841,7 +841,7 @@
         <v>1215.833333333333</v>
       </c>
       <c r="C12" s="3">
-        <v>4.52008791457193</v>
+        <v>4.520087914571929</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -852,7 +852,7 @@
         <v>1003.333333333333</v>
       </c>
       <c r="C13" s="3">
-        <v>2.327125813468715</v>
+        <v>2.327125813468714</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -863,7 +863,7 @@
         <v>966.9444444444445</v>
       </c>
       <c r="C14" s="3">
-        <v>3.63338381135134</v>
+        <v>3.633383811351339</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -874,7 +874,7 @@
         <v>2408.055555555556</v>
       </c>
       <c r="C15" s="3">
-        <v>1.940028840493859</v>
+        <v>1.940028840493857</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -885,7 +885,7 @@
         <v>704.5</v>
       </c>
       <c r="C16" s="3">
-        <v>2.838654908492099</v>
+        <v>2.838654908492098</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -896,7 +896,7 @@
         <v>645.2777777777778</v>
       </c>
       <c r="C17" s="3">
-        <v>0.8796179759578744</v>
+        <v>0.8796179759578739</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -907,7 +907,7 @@
         <v>7539.722222222223</v>
       </c>
       <c r="C18" s="3">
-        <v>2.369143003552927</v>
+        <v>2.369143003552926</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -918,7 +918,7 @@
         <v>366.0555555555555</v>
       </c>
       <c r="C19" s="3">
-        <v>5.145604421258338</v>
+        <v>5.145604421258336</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -929,7 +929,7 @@
         <v>2289.888888888889</v>
       </c>
       <c r="C20" s="3">
-        <v>2.114770802958087</v>
+        <v>2.114770802958086</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -962,7 +962,7 @@
         <v>1404.611111111111</v>
       </c>
       <c r="C23" s="3">
-        <v>3.339439589950416</v>
+        <v>3.339439589950415</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -973,7 +973,7 @@
         <v>1308.944444444444</v>
       </c>
       <c r="C24" s="3">
-        <v>2.978555887229456</v>
+        <v>2.978555887229455</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -995,7 +995,7 @@
         <v>3735.055555555556</v>
       </c>
       <c r="C26" s="3">
-        <v>1.624458607049496</v>
+        <v>1.624458607049495</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1006,7 +1006,7 @@
         <v>19142.27777777778</v>
       </c>
       <c r="C27" s="3">
-        <v>0.9990234685779522</v>
+        <v>0.9990234685779518</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1028,7 +1028,7 @@
         <v>1108.333333333333</v>
       </c>
       <c r="C29" s="3">
-        <v>4.379423800184783</v>
+        <v>4.379423800184782</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1039,7 +1039,7 @@
         <v>847.2777777777778</v>
       </c>
       <c r="C30" s="3">
-        <v>2.57203166618099</v>
+        <v>2.572031666180989</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1050,7 +1050,7 @@
         <v>16813.55555555555</v>
       </c>
       <c r="C31" s="3">
-        <v>1.82441677037982</v>
+        <v>1.824416770379819</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1061,7 +1061,7 @@
         <v>1382.111111111111</v>
       </c>
       <c r="C32" s="3">
-        <v>4.898482965635325</v>
+        <v>4.898482965635324</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1072,7 +1072,7 @@
         <v>765.875</v>
       </c>
       <c r="C33" s="3">
-        <v>0.5731196185501006</v>
+        <v>0.5731196185501002</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1083,7 +1083,7 @@
         <v>1598.5</v>
       </c>
       <c r="C34" s="3">
-        <v>0.5343369108736047</v>
+        <v>0.534336910873604</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1094,7 +1094,7 @@
         <v>52043.83333333334</v>
       </c>
       <c r="C35" s="3">
-        <v>0.9589643109472241</v>
+        <v>0.9589643109472237</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1105,7 +1105,7 @@
         <v>721.0555555555555</v>
       </c>
       <c r="C36" s="3">
-        <v>3.327938956505584</v>
+        <v>3.327938956505583</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1116,7 +1116,7 @@
         <v>697</v>
       </c>
       <c r="C37" s="3">
-        <v>1.945810289036112</v>
+        <v>1.945810289036111</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1127,7 +1127,7 @@
         <v>4986.222222222223</v>
       </c>
       <c r="C38" s="3">
-        <v>2.416673700971705</v>
+        <v>2.416673700971704</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1138,7 +1138,7 @@
         <v>5723.611111111111</v>
       </c>
       <c r="C39" s="3">
-        <v>1.509234673336075</v>
+        <v>1.509234673336074</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1171,7 +1171,7 @@
         <v>4127.166666666667</v>
       </c>
       <c r="C42" s="3">
-        <v>2.115583174554906</v>
+        <v>2.115583174554905</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1182,7 +1182,7 @@
         <v>932</v>
       </c>
       <c r="C43" s="3">
-        <v>1.756911632289729</v>
+        <v>1.756911632289728</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1204,7 +1204,7 @@
         <v>1298.388888888889</v>
       </c>
       <c r="C45" s="3">
-        <v>3.176899455564954</v>
+        <v>3.176899455564953</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1215,7 +1215,7 @@
         <v>1161.5</v>
       </c>
       <c r="C46" s="3">
-        <v>4.91099571033046</v>
+        <v>4.910995710330458</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1226,7 +1226,7 @@
         <v>489.0555555555555</v>
       </c>
       <c r="C47" s="3">
-        <v>3.00883816873217</v>
+        <v>3.008838168732169</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1237,7 +1237,7 @@
         <v>1469.222222222222</v>
       </c>
       <c r="C48" s="3">
-        <v>2.720345156539986</v>
+        <v>2.720345156539985</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1248,7 +1248,7 @@
         <v>898.9444444444445</v>
       </c>
       <c r="C49" s="3">
-        <v>8.023132541218962</v>
+        <v>8.023132541218958</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1259,7 +1259,7 @@
         <v>589.5555555555555</v>
       </c>
       <c r="C50" s="3">
-        <v>4.246522363577466</v>
+        <v>4.246522363577464</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1270,7 +1270,7 @@
         <v>1381</v>
       </c>
       <c r="C51" s="3">
-        <v>5.418253715538313</v>
+        <v>5.418253715538312</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1292,7 +1292,7 @@
         <v>4762.055555555556</v>
       </c>
       <c r="C53" s="3">
-        <v>3.2812355530541</v>
+        <v>3.281235553054099</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1303,7 +1303,7 @@
         <v>304.5555555555555</v>
       </c>
       <c r="C54" s="3">
-        <v>5.423905213307879</v>
+        <v>5.423905213307878</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1314,7 +1314,7 @@
         <v>2657.555555555556</v>
       </c>
       <c r="C55" s="3">
-        <v>4.197561285620758</v>
+        <v>4.197561285620757</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1336,7 +1336,7 @@
         <v>65204.44444444445</v>
       </c>
       <c r="C57" s="3">
-        <v>1.277468593367814</v>
+        <v>1.277468593367813</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1347,7 +1347,7 @@
         <v>1029.5</v>
       </c>
       <c r="C58" s="3">
-        <v>0.928371439701003</v>
+        <v>0.9283714397010026</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1358,7 +1358,7 @@
         <v>4244.111111111111</v>
       </c>
       <c r="C59" s="3">
-        <v>1.952990849728096</v>
+        <v>1.952990849728095</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1369,7 +1369,7 @@
         <v>953.5555555555555</v>
       </c>
       <c r="C60" s="3">
-        <v>4.03828616167214</v>
+        <v>4.038286161672139</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1380,7 +1380,7 @@
         <v>1344.444444444444</v>
       </c>
       <c r="C61" s="3">
-        <v>3.921826183576597</v>
+        <v>3.921826183576596</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1391,7 +1391,7 @@
         <v>1676.388888888889</v>
       </c>
       <c r="C62" s="3">
-        <v>2.591569538840901</v>
+        <v>2.5915695388409</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1413,7 +1413,7 @@
         <v>688.2222222222222</v>
       </c>
       <c r="C64" s="3">
-        <v>2.704154469791416</v>
+        <v>2.704154469791415</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1424,7 +1424,7 @@
         <v>1787.444444444444</v>
       </c>
       <c r="C65" s="3">
-        <v>2.554172184965164</v>
+        <v>2.554172184965163</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1435,7 +1435,7 @@
         <v>1955.555555555556</v>
       </c>
       <c r="C66" s="3">
-        <v>3.707019874209064</v>
+        <v>3.707019874209062</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1446,7 +1446,7 @@
         <v>1406.222222222222</v>
       </c>
       <c r="C67" s="3">
-        <v>2.606731384182656</v>
+        <v>2.606731384182655</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1457,7 +1457,7 @@
         <v>1148.666666666667</v>
       </c>
       <c r="C68" s="3">
-        <v>2.967199738267892</v>
+        <v>2.967199738267891</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1468,7 +1468,7 @@
         <v>994.7777777777778</v>
       </c>
       <c r="C69" s="3">
-        <v>5.274725717453603</v>
+        <v>5.274725717453602</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1479,7 +1479,7 @@
         <v>433</v>
       </c>
       <c r="C70" s="3">
-        <v>3.283537035349038</v>
+        <v>3.283537035349037</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1490,7 +1490,7 @@
         <v>15794.88888888889</v>
       </c>
       <c r="C71" s="3">
-        <v>1.732085870349755</v>
+        <v>1.732085870349754</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1501,7 +1501,7 @@
         <v>845.8888888888889</v>
       </c>
       <c r="C72" s="3">
-        <v>1.809890164114267</v>
+        <v>1.809890164114266</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1512,7 +1512,7 @@
         <v>1314.277777777778</v>
       </c>
       <c r="C73" s="3">
-        <v>1.865748618876329</v>
+        <v>1.865748618876328</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1523,7 +1523,7 @@
         <v>360.3333333333333</v>
       </c>
       <c r="C74" s="3">
-        <v>3.257262687746989</v>
+        <v>3.257262687746988</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1556,7 +1556,7 @@
         <v>1208.611111111111</v>
       </c>
       <c r="C77" s="3">
-        <v>4.085181848712214</v>
+        <v>4.085181848712213</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1589,7 +1589,7 @@
         <v>1820.388888888889</v>
       </c>
       <c r="C80" s="3">
-        <v>0.5713111538130027</v>
+        <v>0.5713111538130025</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1600,7 +1600,7 @@
         <v>1480.333333333333</v>
       </c>
       <c r="C81" s="3">
-        <v>1.692927509218714</v>
+        <v>1.692927509218713</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1622,7 +1622,7 @@
         <v>426.5</v>
       </c>
       <c r="C83" s="3">
-        <v>4.635793554937601</v>
+        <v>4.6357935549376</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1633,7 +1633,7 @@
         <v>1599.111111111111</v>
       </c>
       <c r="C84" s="3">
-        <v>2.981145719466403</v>
+        <v>2.981145719466402</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1655,7 +1655,7 @@
         <v>246.4117647058823</v>
       </c>
       <c r="C86" s="3">
-        <v>1.158124226992247</v>
+        <v>1.158124226992246</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1666,7 +1666,7 @@
         <v>812.8333333333334</v>
       </c>
       <c r="C87" s="3">
-        <v>3.336739651606501</v>
+        <v>3.336739651606499</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1677,7 +1677,7 @@
         <v>950.3333333333334</v>
       </c>
       <c r="C88" s="3">
-        <v>2.968406732834276</v>
+        <v>2.968406732834275</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1688,7 +1688,7 @@
         <v>718.3333333333334</v>
       </c>
       <c r="C89" s="3">
-        <v>7.020103735428295</v>
+        <v>7.020103735428293</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1699,7 +1699,7 @@
         <v>1363.166666666667</v>
       </c>
       <c r="C90" s="3">
-        <v>3.418821882174068</v>
+        <v>3.418821882174067</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1721,7 +1721,7 @@
         <v>1087.055555555556</v>
       </c>
       <c r="C92" s="3">
-        <v>4.759575287918112</v>
+        <v>4.759575287918111</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1732,7 +1732,7 @@
         <v>1021.222222222222</v>
       </c>
       <c r="C93" s="3">
-        <v>6.007627490035413</v>
+        <v>6.007627490035412</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1743,7 +1743,7 @@
         <v>2075.555555555556</v>
       </c>
       <c r="C94" s="3">
-        <v>2.260271692479445</v>
+        <v>2.260271692479444</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1754,7 +1754,7 @@
         <v>5576.888888888889</v>
       </c>
       <c r="C95" s="3">
-        <v>1.58632640112353</v>
+        <v>1.586326401123529</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1776,7 +1776,7 @@
         <v>349.6666666666667</v>
       </c>
       <c r="C97" s="3">
-        <v>2.678940404510246</v>
+        <v>2.678940404510245</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1787,7 +1787,7 @@
         <v>4738.722222222223</v>
       </c>
       <c r="C98" s="3">
-        <v>2.02089813747905</v>
+        <v>2.020898137479049</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1798,7 +1798,7 @@
         <v>429.7222222222222</v>
       </c>
       <c r="C99" s="3">
-        <v>2.454632666991827</v>
+        <v>2.454632666991826</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1809,7 +1809,7 @@
         <v>4262.444444444444</v>
       </c>
       <c r="C100" s="3">
-        <v>1.518729168682849</v>
+        <v>1.518729168682848</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1820,7 +1820,7 @@
         <v>1411.222222222222</v>
       </c>
       <c r="C101" s="3">
-        <v>2.741347663741912</v>
+        <v>2.741347663741911</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1831,7 +1831,7 @@
         <v>1071.666666666667</v>
       </c>
       <c r="C102" s="3">
-        <v>3.382878491978186</v>
+        <v>3.382878491978184</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1842,7 +1842,7 @@
         <v>4690</v>
       </c>
       <c r="C103" s="3">
-        <v>1.939948131515449</v>
+        <v>1.939948131515448</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1853,7 +1853,7 @@
         <v>610.0555555555555</v>
       </c>
       <c r="C104" s="3">
-        <v>4.675489641386827</v>
+        <v>4.675489641386826</v>
       </c>
     </row>
     <row r="105" spans="1:3">

</xml_diff>